<commit_message>
changes for week ending 25th Mar
</commit_message>
<xml_diff>
--- a/TestData/TestData_iNeo.xlsx
+++ b/TestData/TestData_iNeo.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Iflightneo_github\Iflightneo_github\iFlightNeo\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Iflightneo_latest2\iFlightNeo\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8410305-038C-4B48-8675-ECAE0820F913}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96E00F82-2D25-4798-90C9-B64E862F05CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -292,7 +292,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1254" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1287" uniqueCount="225">
   <si>
     <t>ScriptName</t>
   </si>
@@ -962,6 +962,18 @@
   </si>
   <si>
     <t>26-Mar-2022</t>
+  </si>
+  <si>
+    <t>NeoOps_AAF_TC057</t>
+  </si>
+  <si>
+    <t>53</t>
+  </si>
+  <si>
+    <t>08-Apr-2022</t>
+  </si>
+  <si>
+    <t>3018,3000</t>
   </si>
 </sst>
 </file>
@@ -1600,13 +1612,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:XCA53"/>
+  <dimension ref="A1:XCA54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="102" zoomScaleNormal="102" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C30" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J53" sqref="J53"/>
+      <selection pane="bottomRight" activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5333,7 +5345,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="49" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
         <v>182</v>
       </c>
@@ -5359,7 +5371,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="50" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
         <v>184</v>
       </c>
@@ -5385,7 +5397,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="51" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
         <v>186</v>
       </c>
@@ -5411,7 +5423,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="52" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
         <v>187</v>
       </c>
@@ -5434,7 +5446,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="53" spans="1:30" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:33" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="24" t="s">
         <v>217</v>
       </c>
@@ -5523,13 +5535,114 @@
         <v>38</v>
       </c>
       <c r="AD53" s="23" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="54" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A54" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="B54" s="23" t="s">
+        <v>221</v>
+      </c>
+      <c r="C54" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="D54" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="E54" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="F54" s="25" t="s">
+        <v>209</v>
+      </c>
+      <c r="G54" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="H54" s="23" t="s">
+        <v>223</v>
+      </c>
+      <c r="I54" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J54" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="K54" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="L54" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="M54" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="N54" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="O54" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="P54" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q54" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="R54" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="S54" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="T54" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="U54" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="V54" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="W54" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="X54" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y54" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z54" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA54" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB54" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC54" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="AD54" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="AE54" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="AF54" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="AG54" s="23" t="s">
         <v>38</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D24:D29 C2:C30 C39 C53:D53" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D24:D29 C2:C30 C39 C53:D54" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Chrome,Firefox,Edge"</formula1>
     </dataValidation>
   </dataValidations>
@@ -5626,10 +5739,12 @@
     <hyperlink ref="F23" r:id="rId90" xr:uid="{45923769-6036-4C93-BCBE-4D0631E2641F}"/>
     <hyperlink ref="D53" r:id="rId91" xr:uid="{9839F7FC-A6C1-4676-9868-427ADBC15587}"/>
     <hyperlink ref="F53" r:id="rId92" xr:uid="{02DC16D4-2D65-4CA8-9EC3-66B1413BCC6F}"/>
+    <hyperlink ref="D54" r:id="rId93" xr:uid="{1FE02F76-38A2-4C68-BFC0-D7E12E9BD098}"/>
+    <hyperlink ref="F54" r:id="rId94" xr:uid="{FF6B35B6-95FF-45AB-BB83-9500D566875E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId93"/>
-  <legacyDrawing r:id="rId94"/>
+  <pageSetup orientation="portrait" r:id="rId95"/>
+  <legacyDrawing r:id="rId96"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
script improvements and all messages for interface scripts
</commit_message>
<xml_diff>
--- a/TestData/TestData_iNeo.xlsx
+++ b/TestData/TestData_iNeo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\0903B8744\git\iFlightNeov28Mar\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\eclipse-workspace\iFlightNeo_GitProject\iFlightNeov28Mar\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41035B91-CE02-407F-A163-E8DFEE9E6C38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66E3953E-2030-4E3A-B850-17DC5972106C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-165" yWindow="-165" windowWidth="29130" windowHeight="15930" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Driver" sheetId="2" state="hidden" r:id="rId1"/>
@@ -292,7 +292,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1318" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1318" uniqueCount="247">
   <si>
     <t>ScriptName</t>
   </si>
@@ -880,18 +880,12 @@
     <t>A6-EJA</t>
   </si>
   <si>
-    <t>3401</t>
-  </si>
-  <si>
     <t>3402</t>
   </si>
   <si>
     <t>3403</t>
   </si>
   <si>
-    <t>3404</t>
-  </si>
-  <si>
     <t>3405</t>
   </si>
   <si>
@@ -1043,6 +1037,9 @@
   </si>
   <si>
     <t>3000</t>
+  </si>
+  <si>
+    <t>3805</t>
   </si>
 </sst>
 </file>
@@ -1594,15 +1591,15 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.26953125" customWidth="1"/>
-    <col min="4" max="5" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" customWidth="1"/>
+    <col min="4" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -1616,7 +1613,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1630,7 +1627,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1642,7 +1639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1654,7 +1651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1666,7 +1663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1697,41 +1694,41 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C28" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H64" sqref="H64"/>
+      <selection pane="bottomRight" activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.26953125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.26953125" style="18" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.28515625" style="18" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="54" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.26953125" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.453125" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.54296875" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.26953125" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.26953125" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.81640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="4.7265625" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.26953125" style="4" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.26953125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.28515625" style="4" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="7" style="4" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="11.7265625" style="4" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="5.81640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.453125" style="4" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.7265625" style="4" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="8.26953125" style="4" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="14.1796875" style="4" bestFit="1" customWidth="1"/>
-    <col min="23" max="24" width="16.26953125" style="4" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="14.54296875" style="4" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="16.1796875" style="4" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="15.453125" style="4" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="14.26953125" style="4" bestFit="1" customWidth="1"/>
-    <col min="29" max="16384" width="9.1796875" style="4"/>
+    <col min="16" max="17" width="11.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="5.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="16.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="16.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="15.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="14.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="29" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -1817,16 +1814,16 @@
         <v>99</v>
       </c>
       <c r="AC1" s="17" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="AD1" s="17" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="AE1" s="17" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.35">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -1840,10 +1837,10 @@
         <v>46</v>
       </c>
       <c r="E2" s="23" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="F2" s="26" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>41</v>
@@ -1912,7 +1909,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" s="20">
         <v>2</v>
       </c>
@@ -1929,7 +1926,7 @@
         <v>47</v>
       </c>
       <c r="F3" s="25" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="G3" s="5" t="s">
         <v>60</v>
@@ -1998,7 +1995,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>3</v>
       </c>
@@ -2015,7 +2012,7 @@
         <v>47</v>
       </c>
       <c r="F4" s="25" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>40</v>
@@ -2084,7 +2081,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" s="20">
         <v>4</v>
       </c>
@@ -2101,7 +2098,7 @@
         <v>47</v>
       </c>
       <c r="F5" s="25" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="G5" s="5" t="s">
         <v>54</v>
@@ -2170,7 +2167,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>5</v>
       </c>
@@ -2187,7 +2184,7 @@
         <v>47</v>
       </c>
       <c r="F6" s="25" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>36</v>
@@ -2256,7 +2253,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" s="20">
         <v>6</v>
       </c>
@@ -2273,7 +2270,7 @@
         <v>47</v>
       </c>
       <c r="F7" s="25" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="G7" s="5" t="s">
         <v>50</v>
@@ -2342,7 +2339,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>7</v>
       </c>
@@ -2359,7 +2356,7 @@
         <v>47</v>
       </c>
       <c r="F8" s="25" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="G8" s="7" t="s">
         <v>107</v>
@@ -2428,7 +2425,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" s="20">
         <v>8</v>
       </c>
@@ -2445,7 +2442,7 @@
         <v>47</v>
       </c>
       <c r="F9" s="25" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="G9" s="7" t="s">
         <v>64</v>
@@ -2514,7 +2511,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>9</v>
       </c>
@@ -2531,7 +2528,7 @@
         <v>47</v>
       </c>
       <c r="F10" s="25" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="G10" s="7" t="s">
         <v>58</v>
@@ -2600,7 +2597,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11" s="20">
         <v>10</v>
       </c>
@@ -2617,7 +2614,7 @@
         <v>47</v>
       </c>
       <c r="F11" s="25" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>36</v>
@@ -2686,7 +2683,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
         <v>11</v>
       </c>
@@ -2772,7 +2769,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A13" s="20">
         <v>12</v>
       </c>
@@ -2789,7 +2786,7 @@
         <v>47</v>
       </c>
       <c r="F13" s="25" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="G13" s="18" t="s">
         <v>36</v>
@@ -2858,7 +2855,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:31" s="18" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:31" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
         <v>13</v>
       </c>
@@ -2875,7 +2872,7 @@
         <v>47</v>
       </c>
       <c r="F14" s="25" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="G14" s="18" t="s">
         <v>36</v>
@@ -2944,7 +2941,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A15" s="20">
         <v>14</v>
       </c>
@@ -2961,7 +2958,7 @@
         <v>47</v>
       </c>
       <c r="F15" s="25" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="G15" s="18" t="s">
         <v>36</v>
@@ -3030,7 +3027,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A16" s="7">
         <v>15</v>
       </c>
@@ -3047,7 +3044,7 @@
         <v>47</v>
       </c>
       <c r="F16" s="25" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="G16" s="18" t="s">
         <v>36</v>
@@ -3116,7 +3113,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:29 16301:16301" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:29 16301:16301" x14ac:dyDescent="0.25">
       <c r="A17" s="20">
         <v>16</v>
       </c>
@@ -3133,7 +3130,7 @@
         <v>47</v>
       </c>
       <c r="F17" s="25" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="G17" s="18" t="s">
         <v>36</v>
@@ -3202,7 +3199,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:29 16301:16301" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:29 16301:16301" x14ac:dyDescent="0.25">
       <c r="A18" s="7">
         <v>17</v>
       </c>
@@ -3219,7 +3216,7 @@
         <v>47</v>
       </c>
       <c r="F18" s="25" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="G18" s="18" t="s">
         <v>36</v>
@@ -3288,7 +3285,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:29 16301:16301" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:29 16301:16301" x14ac:dyDescent="0.25">
       <c r="A19" s="20">
         <v>18</v>
       </c>
@@ -3305,7 +3302,7 @@
         <v>47</v>
       </c>
       <c r="F19" s="25" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="G19" s="18" t="s">
         <v>36</v>
@@ -3374,7 +3371,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:29 16301:16301" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:29 16301:16301" x14ac:dyDescent="0.25">
       <c r="A20" s="20">
         <v>19</v>
       </c>
@@ -3391,7 +3388,7 @@
         <v>47</v>
       </c>
       <c r="F20" s="25" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="G20" s="7" t="s">
         <v>101</v>
@@ -3460,7 +3457,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="21" spans="1:29 16301:16301" s="18" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:29 16301:16301" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="20">
         <v>20</v>
       </c>
@@ -3477,7 +3474,7 @@
         <v>47</v>
       </c>
       <c r="F21" s="25" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="G21" s="7" t="s">
         <v>101</v>
@@ -3546,7 +3543,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:29 16301:16301" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:29 16301:16301" x14ac:dyDescent="0.25">
       <c r="A22" s="20">
         <v>21</v>
       </c>
@@ -3563,10 +3560,10 @@
         <v>47</v>
       </c>
       <c r="F22" s="25" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="G22" s="24" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="H22" s="23" t="s">
         <v>36</v>
@@ -3575,7 +3572,7 @@
         <v>16</v>
       </c>
       <c r="J22" s="9" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="K22" s="18" t="s">
         <v>36</v>
@@ -3632,11 +3629,11 @@
         <v>36</v>
       </c>
       <c r="AC22" s="4" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="XBY22" s="18"/>
     </row>
-    <row r="23" spans="1:29 16301:16301" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:29 16301:16301" x14ac:dyDescent="0.25">
       <c r="A23" s="20">
         <v>22</v>
       </c>
@@ -3650,10 +3647,10 @@
         <v>46</v>
       </c>
       <c r="E23" s="23" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="F23" s="26" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="G23" s="4" t="s">
         <v>107</v>
@@ -3722,7 +3719,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="24" spans="1:29 16301:16301" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:29 16301:16301" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>116</v>
       </c>
@@ -3739,7 +3736,7 @@
         <v>47</v>
       </c>
       <c r="F24" s="25" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="G24" s="18" t="s">
         <v>36</v>
@@ -3808,7 +3805,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="1:29 16301:16301" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:29 16301:16301" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>117</v>
       </c>
@@ -3825,7 +3822,7 @@
         <v>47</v>
       </c>
       <c r="F25" s="25" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="G25" s="18" t="s">
         <v>36</v>
@@ -3894,7 +3891,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="1:29 16301:16301" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:29 16301:16301" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>118</v>
       </c>
@@ -3911,7 +3908,7 @@
         <v>47</v>
       </c>
       <c r="F26" s="25" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="G26" s="18" t="s">
         <v>36</v>
@@ -3980,7 +3977,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:29 16301:16301" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:29 16301:16301" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>119</v>
       </c>
@@ -3997,7 +3994,7 @@
         <v>47</v>
       </c>
       <c r="F27" s="25" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="G27" s="18" t="s">
         <v>36</v>
@@ -4066,7 +4063,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="28" spans="1:29 16301:16301" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:29 16301:16301" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
         <v>120</v>
       </c>
@@ -4083,7 +4080,7 @@
         <v>47</v>
       </c>
       <c r="F28" s="25" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="G28" s="18" t="s">
         <v>122</v>
@@ -4152,7 +4149,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="29" spans="1:29 16301:16301" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:29 16301:16301" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>130</v>
       </c>
@@ -4169,7 +4166,7 @@
         <v>144</v>
       </c>
       <c r="F29" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="G29" s="4" t="s">
         <v>129</v>
@@ -4238,7 +4235,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="30" spans="1:29 16301:16301" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:29 16301:16301" x14ac:dyDescent="0.25">
       <c r="A30" s="24" t="s">
         <v>135</v>
       </c>
@@ -4255,10 +4252,10 @@
         <v>47</v>
       </c>
       <c r="F30" s="25" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="G30" s="23" t="s">
-        <v>193</v>
+        <v>246</v>
       </c>
       <c r="H30" s="23" t="s">
         <v>36</v>
@@ -4324,7 +4321,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="31" spans="1:29 16301:16301" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:29 16301:16301" x14ac:dyDescent="0.25">
       <c r="A31" s="24" t="s">
         <v>136</v>
       </c>
@@ -4341,10 +4338,10 @@
         <v>47</v>
       </c>
       <c r="F31" s="25" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="G31" s="23" t="s">
-        <v>193</v>
+        <v>246</v>
       </c>
       <c r="H31" s="23" t="s">
         <v>36</v>
@@ -4410,7 +4407,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="32" spans="1:29 16301:16301" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:29 16301:16301" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>137</v>
       </c>
@@ -4427,7 +4424,7 @@
         <v>47</v>
       </c>
       <c r="F32" s="25" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="G32" s="23" t="s">
         <v>36</v>
@@ -4496,7 +4493,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="33" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>139</v>
       </c>
@@ -4513,10 +4510,10 @@
         <v>47</v>
       </c>
       <c r="F33" s="25" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="G33" s="23" t="s">
-        <v>193</v>
+        <v>246</v>
       </c>
       <c r="H33" s="23" t="s">
         <v>36</v>
@@ -4582,7 +4579,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="34" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>141</v>
       </c>
@@ -4599,10 +4596,10 @@
         <v>47</v>
       </c>
       <c r="F34" s="25" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="G34" s="23" t="s">
-        <v>193</v>
+        <v>246</v>
       </c>
       <c r="H34" s="23" t="s">
         <v>36</v>
@@ -4668,7 +4665,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="35" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A35" s="24" t="s">
         <v>146</v>
       </c>
@@ -4685,10 +4682,10 @@
         <v>47</v>
       </c>
       <c r="F35" s="25" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="G35" s="23" t="s">
-        <v>193</v>
+        <v>246</v>
       </c>
       <c r="H35" s="23" t="s">
         <v>36</v>
@@ -4754,7 +4751,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="36" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A36" s="24" t="s">
         <v>149</v>
       </c>
@@ -4840,7 +4837,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="37" spans="1:28" s="23" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:28" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="24" t="s">
         <v>154</v>
       </c>
@@ -4857,16 +4854,16 @@
         <v>47</v>
       </c>
       <c r="F37" s="25" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="G37" s="23" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="K37" s="23" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="38" spans="1:28" s="23" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:28" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="24" t="s">
         <v>156</v>
       </c>
@@ -4883,16 +4880,16 @@
         <v>47</v>
       </c>
       <c r="F38" s="25" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="G38" s="23" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="K38" s="23" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="39" spans="1:28" s="23" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:28" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="24" t="s">
         <v>159</v>
       </c>
@@ -4909,10 +4906,10 @@
         <v>47</v>
       </c>
       <c r="F39" s="25" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="G39" s="23" t="s">
-        <v>196</v>
+        <v>246</v>
       </c>
       <c r="H39" s="23" t="s">
         <v>36</v>
@@ -4978,7 +4975,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="40" spans="1:28" s="23" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:28" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="24" t="s">
         <v>161</v>
       </c>
@@ -4995,16 +4992,16 @@
         <v>47</v>
       </c>
       <c r="F40" s="25" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="G40" s="23" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="K40" s="23" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="41" spans="1:28" s="23" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:28" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="24" t="s">
         <v>163</v>
       </c>
@@ -5021,16 +5018,16 @@
         <v>47</v>
       </c>
       <c r="F41" s="25" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="G41" s="23" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="K41" s="23" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="42" spans="1:28" s="23" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:28" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="24" t="s">
         <v>165</v>
       </c>
@@ -5047,16 +5044,16 @@
         <v>47</v>
       </c>
       <c r="F42" s="25" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="G42" s="23" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="K42" s="23" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="43" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
         <v>166</v>
       </c>
@@ -5073,16 +5070,16 @@
         <v>47</v>
       </c>
       <c r="F43" s="25" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="G43" s="23" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="K43" s="4" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="44" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A44" s="24" t="s">
         <v>169</v>
       </c>
@@ -5099,13 +5096,13 @@
         <v>47</v>
       </c>
       <c r="F44" s="25" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="G44" s="23" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="45" spans="1:28" x14ac:dyDescent="0.35">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="45" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
         <v>171</v>
       </c>
@@ -5122,16 +5119,16 @@
         <v>47</v>
       </c>
       <c r="F45" s="25" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="G45" s="4" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="K45" s="23" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="46" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
         <v>172</v>
       </c>
@@ -5148,16 +5145,16 @@
         <v>47</v>
       </c>
       <c r="F46" s="25" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="G46" s="23" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="K46" s="23" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="47" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
         <v>175</v>
       </c>
@@ -5174,13 +5171,13 @@
         <v>47</v>
       </c>
       <c r="F47" s="25" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="G47" s="23" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="48" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
         <v>177</v>
       </c>
@@ -5197,16 +5194,16 @@
         <v>47</v>
       </c>
       <c r="F48" s="25" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="G48" s="4" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="K48" s="23" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="49" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
         <v>180</v>
       </c>
@@ -5223,16 +5220,16 @@
         <v>47</v>
       </c>
       <c r="F49" s="25" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="G49" s="4" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="K49" s="23" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="50" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
         <v>182</v>
       </c>
@@ -5249,16 +5246,16 @@
         <v>47</v>
       </c>
       <c r="F50" s="25" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="G50" s="23" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="K50" s="23" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="51" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
         <v>184</v>
       </c>
@@ -5275,16 +5272,16 @@
         <v>47</v>
       </c>
       <c r="F51" s="25" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="G51" s="23" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="K51" s="23" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="52" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
         <v>185</v>
       </c>
@@ -5301,18 +5298,18 @@
         <v>47</v>
       </c>
       <c r="F52" s="25" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="G52" s="23" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="53" spans="1:31" s="23" customFormat="1" x14ac:dyDescent="0.35">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="53" spans="1:31" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="24" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B53" s="23" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C53" s="23" t="s">
         <v>91</v>
@@ -5324,13 +5321,13 @@
         <v>47</v>
       </c>
       <c r="F53" s="25" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="G53" s="23" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="H53" s="23" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="I53" s="23" t="s">
         <v>16</v>
@@ -5393,12 +5390,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="54" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B54" s="23" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C54" s="23" t="s">
         <v>91</v>
@@ -5410,19 +5407,19 @@
         <v>47</v>
       </c>
       <c r="F54" s="25" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="G54" s="4" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="H54" s="23" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="I54" s="4" t="s">
         <v>16</v>
       </c>
       <c r="J54" s="4" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="K54" s="4" t="s">
         <v>36</v>
@@ -5488,12 +5485,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="55" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A55" s="24" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B55" s="23" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C55" s="23" t="s">
         <v>91</v>
@@ -5502,21 +5499,21 @@
         <v>46</v>
       </c>
       <c r="E55" s="23" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="F55" s="26" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="G55" s="23" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="56" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A56" s="24" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B56" s="27" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C56" s="23" t="s">
         <v>91</v>
@@ -5525,21 +5522,21 @@
         <v>46</v>
       </c>
       <c r="E56" s="23" t="s">
+        <v>222</v>
+      </c>
+      <c r="F56" s="26" t="s">
+        <v>205</v>
+      </c>
+      <c r="G56" s="23" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="57" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A57" s="24" t="s">
+        <v>227</v>
+      </c>
+      <c r="B57" s="4" t="s">
         <v>224</v>
-      </c>
-      <c r="F56" s="26" t="s">
-        <v>207</v>
-      </c>
-      <c r="G56" s="23" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="57" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A57" s="24" t="s">
-        <v>229</v>
-      </c>
-      <c r="B57" s="4" t="s">
-        <v>226</v>
       </c>
       <c r="C57" s="23" t="s">
         <v>91</v>
@@ -5548,10 +5545,10 @@
         <v>46</v>
       </c>
       <c r="E57" s="23" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="F57" s="26" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="G57" s="23" t="s">
         <v>36</v>
@@ -5623,18 +5620,18 @@
         <v>36</v>
       </c>
       <c r="AD57" s="28" t="s">
+        <v>230</v>
+      </c>
+      <c r="AE57" s="25" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="58" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A58" s="24" t="s">
         <v>232</v>
       </c>
-      <c r="AE57" s="25" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="58" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A58" s="24" t="s">
-        <v>234</v>
-      </c>
       <c r="B58" s="4" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C58" s="23" t="s">
         <v>91</v>
@@ -5643,18 +5640,18 @@
         <v>46</v>
       </c>
       <c r="E58" s="23" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="F58" s="26" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="59" spans="1:31" s="23" customFormat="1" x14ac:dyDescent="0.35">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="59" spans="1:31" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="24" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B59" s="27" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C59" s="23" t="s">
         <v>91</v>
@@ -5663,18 +5660,18 @@
         <v>46</v>
       </c>
       <c r="E59" s="23" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="F59" s="26" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="60" spans="1:31" x14ac:dyDescent="0.35">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="60" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C60" s="23" t="s">
         <v>91</v>
@@ -5683,16 +5680,16 @@
         <v>46</v>
       </c>
       <c r="E60" s="23" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="F60" s="26" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="G60" s="4" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="H60" s="23" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="I60" s="23" t="s">
         <v>16</v>
@@ -5764,12 +5761,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="61" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C61" s="23" t="s">
         <v>91</v>
@@ -5778,21 +5775,21 @@
         <v>46</v>
       </c>
       <c r="E61" s="23" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="F61" s="26" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="K61" s="4" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="62" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A62" s="24" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="62" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A62" s="24" t="s">
-        <v>244</v>
-      </c>
       <c r="B62" s="23" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C62" s="23" t="s">
         <v>91</v>
@@ -5801,31 +5798,31 @@
         <v>46</v>
       </c>
       <c r="E62" s="23" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="F62" s="26" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="G62" s="4" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="H62" s="23" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="I62" s="4" t="s">
         <v>16</v>
       </c>
       <c r="J62" s="4" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="K62" s="23" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="T62" s="4" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="63" spans="1:31" x14ac:dyDescent="0.35">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="63" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B63" s="23"/>
     </row>
   </sheetData>
@@ -5962,12 +5959,12 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="37.1796875" customWidth="1"/>
+    <col min="2" max="2" width="37.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>65</v>
       </c>
@@ -5975,7 +5972,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -5983,7 +5980,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -5991,7 +5988,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -5999,7 +5996,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -6007,7 +6004,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>

</xml_diff>